<commit_message>
Add xlsx Threat Actor Info
Load threat actor data from an excel sheet which can be modified by users without needing to re-build the Anylogic model, which would require them to have a license. Also, change output to visualize nodes as compromised if they are compromised one or more times, rather than in greater than 50 percent of attack run.
</commit_message>
<xml_diff>
--- a/model/threat_actor_inputs.xlsx
+++ b/model/threat_actor_inputs.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Models\cyberattack-simulation\model-inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Models\cyberattack-simulation\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC2472E-0B5D-41C7-97E0-8113A672083E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCDB35CC-39E2-42FB-8EA9-7FCC0C2B1AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6ED20923-A898-4EA5-9B2B-D5274E045E7C}"/>
+    <workbookView xWindow="4095" yWindow="1020" windowWidth="23715" windowHeight="11385" xr2:uid="{655A996C-7B20-495A-8257-2AF7B3356DDC}"/>
   </bookViews>
   <sheets>
-    <sheet name="attacker_types1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,6 +37,24 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
+    <t>attacker_id</t>
+  </si>
+  <si>
+    <t>attacker_name</t>
+  </si>
+  <si>
+    <t>non_breach_ratio</t>
+  </si>
+  <si>
+    <t>non_breach_n</t>
+  </si>
+  <si>
+    <t>attack_ratio</t>
+  </si>
+  <si>
+    <t>attack_n</t>
+  </si>
+  <si>
     <t>OrganizedCrime</t>
   </si>
   <si>
@@ -59,24 +77,6 @@
   </si>
   <si>
     <t>Competitor</t>
-  </si>
-  <si>
-    <t>attacker_id</t>
-  </si>
-  <si>
-    <t>attacker_name</t>
-  </si>
-  <si>
-    <t>non_breach_ratio</t>
-  </si>
-  <si>
-    <t>non_breach_n</t>
-  </si>
-  <si>
-    <t>attack_ratio</t>
-  </si>
-  <si>
-    <t>attack_n</t>
   </si>
 </sst>
 </file>
@@ -112,9 +112,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,140 +427,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0FA8B4-7ADB-44B3-AF05-8B22F6C5B327}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5CA49C-4EFB-48E5-9F7F-E01756387A5F}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="1" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
         <v>0.182</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>570</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2">
         <v>0.13100000000000001</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2">
         <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
         <v>0.53</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>447</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>3.0800000000000001E-2</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
         <v>0.1051</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>257</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
         <v>6.6400000000000001E-3</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
         <v>4.6899999999999997E-2</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>64</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
         <v>0.125</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>16</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6">
         <v>2.4499999999999999E-3</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
         <v>7</v>
       </c>
     </row>

</xml_diff>